<commit_message>
Updated "SLS-SLS_Implicit Percent Error.xlsx" with Latest Data
</commit_message>
<xml_diff>
--- a/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/10/SLS-SLS_Implicit Percent Error.xlsx
+++ b/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/10/SLS-SLS_Implicit Percent Error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanel\OneDrive\2021LaneLeeCCIFall2021\Github\MSRESOLVESG\UnitTests\TuningCorrector\test_11 Manual SLS Implicit\10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B381CBA-BE30-4ABF-B5AD-FC906249177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC0677C-4279-4712-8E41-A3F3218EA7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41640" yWindow="225" windowWidth="28800" windowHeight="14520" xr2:uid="{1BE193A6-CF44-4ACE-AD4A-AAC9D5EE89E8}"/>
+    <workbookView xWindow="22860" yWindow="1065" windowWidth="28635" windowHeight="14520" xr2:uid="{1BE193A6-CF44-4ACE-AD4A-AAC9D5EE89E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,7 +695,7 @@
   <dimension ref="A2:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,14 +844,14 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>0.71488794869381844</v>
+        <v>0.83081572400000003</v>
       </c>
       <c r="C8" s="3">
         <v>0.83083923630596501</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D15" si="0">((B8-C8)/C8)*100</f>
-        <v>-13.955923426014794</v>
+        <v>-2.8299465092089414E-3</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>

</xml_diff>